<commit_message>
Changes to be committed: deleted:    data/2024Q2_29012025 (1).xlsx modified:   data/2024Q2_29012025.xlsx modified:   pages/Q1-4_2024_Annual_Report.py modified:   pages/Q1_2024_Report.py modified:   pages/Q2_2024_Report.py modified:   pages/Q3_2024_Report.py modified:   pages/Q4_2024_Report.py modified:   utils/charts.py
</commit_message>
<xml_diff>
--- a/data/2024Q2_29012025.xlsx
+++ b/data/2024Q2_29012025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7230B24-72EA-C147-A421-FD8C22BF6D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD8722C-6E44-7F41-A9D6-A61F9BC1584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13760" yWindow="4000" windowWidth="51200" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="criteria for qualitative assess" sheetId="1" r:id="rId1"/>
@@ -964,7 +964,7 @@
   <dimension ref="A1:AD986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -988,7 +988,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F1" s="2" t="s">

</xml_diff>

<commit_message>
modified:   data/2024Q2_29012025.xlsx deleted:    data/2024Q3_03022025 (1).xlsx new file:   data/2024Q3_03022025.xlsx modified:   pages/Q1-4_2024_Annual_Report.py modified:   pages/Q3_2024_Report.py modified:   utils/data_loader.py
</commit_message>
<xml_diff>
--- a/data/2024Q2_29012025.xlsx
+++ b/data/2024Q2_29012025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD8722C-6E44-7F41-A9D6-A61F9BC1584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7CFD5F6-08D9-FE4A-8B0E-B4B828D86D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="4000" windowWidth="51200" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="1740" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="criteria for qualitative assess" sheetId="1" r:id="rId1"/>
@@ -297,9 +297,6 @@
     <t>posted by 1 X user</t>
   </si>
   <si>
-    <t>31.06.2024</t>
-  </si>
-  <si>
     <t>Conditions of women holding management positions in Poland</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
   </si>
   <si>
     <t>Economic and Regional Studies / Studia Ekonomiczne i Regionalne</t>
-  </si>
-  <si>
-    <t>31.06.2025</t>
   </si>
   <si>
     <t>https://sciendo.com/article/10.2478/ers-2024-0016</t>
@@ -484,6 +478,12 @@
   </si>
   <si>
     <t>name of the institution</t>
+  </si>
+  <si>
+    <t>30.06.2024</t>
+  </si>
+  <si>
+    <t>30.06.2025</t>
   </si>
 </sst>
 </file>
@@ -964,7 +964,7 @@
   <dimension ref="A1:AD986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -989,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1654,22 +1654,22 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="C12" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="23" t="s">
         <v>88</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>89</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>40</v>
@@ -1719,22 +1719,22 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="F13" s="26" t="s">
         <v>88</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>89</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>48</v>
@@ -29888,17 +29888,17 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -29908,7 +29908,7 @@
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -29928,12 +29928,12 @@
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30958,104 +30958,104 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="D1" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="28" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="B3" s="28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="C3" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="D3" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C4" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>105</v>
+      <c r="B5" s="28" t="s">
+        <v>110</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="C5" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>110</v>
+      <c r="D5" s="28" t="s">
+        <v>103</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="28" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="28" t="s">
+      <c r="B6" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="C6" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>116</v>
-      </c>
       <c r="D6" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31067,7 +31067,7 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32083,7 +32083,7 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33115,52 +33115,52 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="28" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="B2" s="28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="C2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="D2" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="28" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="B3" s="28" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="C3" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="D3" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="28" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="B4" s="28" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -34181,7 +34181,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -34189,7 +34189,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -34197,7 +34197,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -35219,7 +35219,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -35227,15 +35227,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -36255,15 +36255,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="28">
         <v>0.4</v>
@@ -36271,7 +36271,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" s="28">
         <v>0.2</v>
@@ -36279,7 +36279,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="28">
         <v>0.2</v>
@@ -36287,7 +36287,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B5" s="28">
         <v>0.1</v>
@@ -36295,7 +36295,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" s="28">
         <v>0.1</v>

</xml_diff>